<commit_message>
Finish 1st Notebook + Solve OrdinalEncoded
</commit_message>
<xml_diff>
--- a/[ML]_Project_EDAOutputs_Group33/Tables/Descriptive_Statistics_Numerical.xlsx
+++ b/[ML]_Project_EDAOutputs_Group33/Tables/Descriptive_Statistics_Numerical.xlsx
@@ -516,10 +516,10 @@
         <v>117</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.04057998007326515</v>
+        <v>-0.04</v>
       </c>
       <c r="K2" t="n">
-        <v>-0.4254860373414626</v>
+        <v>-0.43</v>
       </c>
     </row>
     <row r="3">
@@ -553,10 +553,10 @@
         <v>2828079</v>
       </c>
       <c r="J3" t="n">
-        <v>378.9792720672111</v>
+        <v>378.98</v>
       </c>
       <c r="K3" t="n">
-        <v>160021.0394837141</v>
+        <v>160021.04</v>
       </c>
     </row>
     <row r="4">
@@ -590,10 +590,10 @@
         <v>2018</v>
       </c>
       <c r="J4" t="n">
-        <v>-4.325518936569753</v>
+        <v>-4.33</v>
       </c>
       <c r="K4" t="n">
-        <v>16.73425817911194</v>
+        <v>16.73</v>
       </c>
     </row>
     <row r="5">
@@ -627,10 +627,10 @@
         <v>73</v>
       </c>
       <c r="J5" t="n">
-        <v>2.594615719121655</v>
+        <v>2.59</v>
       </c>
       <c r="K5" t="n">
-        <v>13.21382061495355</v>
+        <v>13.21</v>
       </c>
     </row>
     <row r="6">
@@ -664,10 +664,10 @@
         <v>92</v>
       </c>
       <c r="J6" t="n">
-        <v>0.1828337601217862</v>
+        <v>0.18</v>
       </c>
       <c r="K6" t="n">
-        <v>-0.489383310917082</v>
+        <v>-0.49</v>
       </c>
     </row>
     <row r="7">
@@ -701,10 +701,10 @@
         <v>99</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.1301822958004472</v>
+        <v>-0.13</v>
       </c>
       <c r="K7" t="n">
-        <v>-1.025207333041206</v>
+        <v>-1.03</v>
       </c>
     </row>
     <row r="8">
@@ -738,10 +738,10 @@
         <v>91</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.03814939587830273</v>
+        <v>-0.04</v>
       </c>
       <c r="K8" t="n">
-        <v>-0.655539059548508</v>
+        <v>-0.66</v>
       </c>
     </row>
     <row r="9">
@@ -775,10 +775,10 @@
         <v>99</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.07529929200888667</v>
+        <v>-0.08</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4103836418862441</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="10">
@@ -812,10 +812,10 @@
         <v>6</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.003529432849922167</v>
+        <v>-0</v>
       </c>
       <c r="K10" t="n">
-        <v>-1.250324052592594</v>
+        <v>-1.25</v>
       </c>
     </row>
     <row r="11">
@@ -849,10 +849,10 @@
         <v>1</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.7414548596952124</v>
+        <v>-0.74</v>
       </c>
       <c r="K11" t="n">
-        <v>-1.45024974395261</v>
+        <v>-1.45</v>
       </c>
     </row>
     <row r="12">
@@ -886,10 +886,10 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>-1.078378146892873</v>
+        <v>-1.08</v>
       </c>
       <c r="K12" t="n">
-        <v>-0.8371034889208162</v>
+        <v>-0.84</v>
       </c>
     </row>
     <row r="13">
@@ -923,10 +923,10 @@
         <v>2018</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.1525571382712453</v>
+        <v>-0.15</v>
       </c>
       <c r="K13" t="n">
-        <v>-0.7091714615534817</v>
+        <v>-0.71</v>
       </c>
     </row>
     <row r="14">
@@ -960,10 +960,10 @@
         <v>122</v>
       </c>
       <c r="J14" t="n">
-        <v>0.1624434902151317</v>
+        <v>0.16</v>
       </c>
       <c r="K14" t="n">
-        <v>-0.7109711889124104</v>
+        <v>-0.71</v>
       </c>
     </row>
     <row r="15">
@@ -997,10 +997,10 @@
         <v>1</v>
       </c>
       <c r="J15" t="n">
-        <v>0.5576669309507982</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="K15" t="n">
-        <v>-1.689013478933885</v>
+        <v>-1.69</v>
       </c>
     </row>
     <row r="16">
@@ -1034,10 +1034,10 @@
         <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>1.274120939611296</v>
+        <v>1.27</v>
       </c>
       <c r="K16" t="n">
-        <v>-0.3766171434515866</v>
+        <v>-0.38</v>
       </c>
     </row>
     <row r="17">
@@ -1071,10 +1071,10 @@
         <v>2023</v>
       </c>
       <c r="J17" t="n">
-        <v>-10.31601765079053</v>
+        <v>-10.32</v>
       </c>
       <c r="K17" t="n">
-        <v>159.1287006858477</v>
+        <v>159.13</v>
       </c>
     </row>
     <row r="18">
@@ -1108,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.01776812039989087</v>
+        <v>-0.02</v>
       </c>
       <c r="K18" t="n">
-        <v>-1.22546353045317</v>
+        <v>-1.23</v>
       </c>
     </row>
     <row r="19">
@@ -1145,10 +1145,10 @@
         <v>31</v>
       </c>
       <c r="J19" t="n">
-        <v>0.03438260315859069</v>
+        <v>0.03</v>
       </c>
       <c r="K19" t="n">
-        <v>-1.179777769403859</v>
+        <v>-1.18</v>
       </c>
     </row>
     <row r="20">
@@ -1182,10 +1182,10 @@
         <v>6</v>
       </c>
       <c r="J20" t="n">
-        <v>0.2727320388821173</v>
+        <v>0.27</v>
       </c>
       <c r="K20" t="n">
-        <v>-0.9367278364870999</v>
+        <v>-0.9399999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -1219,10 +1219,10 @@
         <v>2022</v>
       </c>
       <c r="J21" t="n">
-        <v>-0.09527774954980402</v>
+        <v>-0.1</v>
       </c>
       <c r="K21" t="n">
-        <v>-1.470837874825765</v>
+        <v>-1.47</v>
       </c>
     </row>
     <row r="22">
@@ -1256,10 +1256,10 @@
         <v>12</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.01611757658106506</v>
+        <v>-0.02</v>
       </c>
       <c r="K22" t="n">
-        <v>-1.215372600554929</v>
+        <v>-1.22</v>
       </c>
     </row>
     <row r="23">
@@ -1293,10 +1293,10 @@
         <v>31</v>
       </c>
       <c r="J23" t="n">
-        <v>0.02325740378663208</v>
+        <v>0.02</v>
       </c>
       <c r="K23" t="n">
-        <v>-1.176738543524942</v>
+        <v>-1.18</v>
       </c>
     </row>
     <row r="24">
@@ -1330,10 +1330,10 @@
         <v>6</v>
       </c>
       <c r="J24" t="n">
-        <v>0.04444936303314442</v>
+        <v>0.04</v>
       </c>
       <c r="K24" t="n">
-        <v>-1.243473588681407</v>
+        <v>-1.24</v>
       </c>
     </row>
     <row r="25">
@@ -1367,10 +1367,10 @@
         <v>2024</v>
       </c>
       <c r="J25" t="n">
-        <v>-7.187660341337669</v>
+        <v>-7.19</v>
       </c>
       <c r="K25" t="n">
-        <v>129.0983054440174</v>
+        <v>129.1</v>
       </c>
     </row>
     <row r="26">
@@ -1404,10 +1404,10 @@
         <v>12</v>
       </c>
       <c r="J26" t="n">
-        <v>-0.01260263651871376</v>
+        <v>-0.01</v>
       </c>
       <c r="K26" t="n">
-        <v>-1.219441395928152</v>
+        <v>-1.22</v>
       </c>
     </row>
     <row r="27">
@@ -1441,10 +1441,10 @@
         <v>31</v>
       </c>
       <c r="J27" t="n">
-        <v>0.0243391605746958</v>
+        <v>0.02</v>
       </c>
       <c r="K27" t="n">
-        <v>-1.175540520059992</v>
+        <v>-1.18</v>
       </c>
     </row>
     <row r="28">
@@ -1478,10 +1478,10 @@
         <v>6</v>
       </c>
       <c r="J28" t="n">
-        <v>0.07893099741117733</v>
+        <v>0.08</v>
       </c>
       <c r="K28" t="n">
-        <v>-1.065677256910117</v>
+        <v>-1.07</v>
       </c>
     </row>
     <row r="29">
@@ -1515,10 +1515,10 @@
         <v>2024</v>
       </c>
       <c r="J29" t="n">
-        <v>-0.1038846515829908</v>
+        <v>-0.1</v>
       </c>
       <c r="K29" t="n">
-        <v>6.365679459607007</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="30">
@@ -1552,10 +1552,10 @@
         <v>12</v>
       </c>
       <c r="J30" t="n">
-        <v>0.01380246193554395</v>
+        <v>0.01</v>
       </c>
       <c r="K30" t="n">
-        <v>-1.214989522370881</v>
+        <v>-1.21</v>
       </c>
     </row>
     <row r="31">
@@ -1589,10 +1589,10 @@
         <v>31</v>
       </c>
       <c r="J31" t="n">
-        <v>0.01531080041798987</v>
+        <v>0.02</v>
       </c>
       <c r="K31" t="n">
-        <v>-1.180649290465092</v>
+        <v>-1.18</v>
       </c>
     </row>
     <row r="32">
@@ -1626,10 +1626,10 @@
         <v>6</v>
       </c>
       <c r="J32" t="n">
-        <v>0.2349838695251223</v>
+        <v>0.23</v>
       </c>
       <c r="K32" t="n">
-        <v>-0.8300572918861837</v>
+        <v>-0.83</v>
       </c>
     </row>
     <row r="33">
@@ -1663,10 +1663,10 @@
         <v>2024</v>
       </c>
       <c r="J33" t="n">
-        <v>0.07680632300198918</v>
+        <v>0.08</v>
       </c>
       <c r="K33" t="n">
-        <v>-0.7833923980671762</v>
+        <v>-0.78</v>
       </c>
     </row>
     <row r="34">
@@ -1700,10 +1700,10 @@
         <v>12</v>
       </c>
       <c r="J34" t="n">
-        <v>0.04927279006297692</v>
+        <v>0.05</v>
       </c>
       <c r="K34" t="n">
-        <v>-1.271649562400561</v>
+        <v>-1.27</v>
       </c>
     </row>
     <row r="35">
@@ -1737,10 +1737,10 @@
         <v>31</v>
       </c>
       <c r="J35" t="n">
-        <v>0.05571318793657582</v>
+        <v>0.06</v>
       </c>
       <c r="K35" t="n">
-        <v>-1.156379166139648</v>
+        <v>-1.16</v>
       </c>
     </row>
     <row r="36">
@@ -1774,10 +1774,10 @@
         <v>4</v>
       </c>
       <c r="J36" t="n">
-        <v>0.01268265619854759</v>
+        <v>0.01</v>
       </c>
       <c r="K36" t="n">
-        <v>-1.390975383929667</v>
+        <v>-1.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>